<commit_message>
update timejournal - add missing title
</commit_message>
<xml_diff>
--- a/docs/time_journal.xlsx
+++ b/docs/time_journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taasane1/Documents/Private/Studium/BSc/4_Semester/WEBLAB/WEBLAB_TechRadar/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EEC248-1EB3-FF48-9F8D-71CFA9DA9F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE182AE5-E9CE-4A4F-A9A7-4985EC9D2A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" xr2:uid="{62EA19C6-2F38-6F4F-910B-35FF851C8F7B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Implementierung</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Stunden</t>
+  </si>
+  <si>
+    <t>Finalisation Projekt</t>
   </si>
 </sst>
 </file>
@@ -444,27 +447,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -494,6 +476,27 @@
     <xf numFmtId="14" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010FBA35-A2D4-884D-8AA6-89BA865457FC}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="106" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,12 +846,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -863,444 +866,446 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="25">
         <v>45691</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="25">
         <v>45691</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="16">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="25">
         <v>45691</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="27">
         <v>45692</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="17">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="27">
         <v>45699</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="25"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="27">
         <v>45692</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="27">
         <v>45702</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="12"/>
-      <c r="D12" s="25"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="28">
         <v>45694</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="28">
         <v>45702</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="25"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="28">
         <v>45693</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="28">
         <v>45702</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="28">
         <v>45696</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="28">
         <v>45696</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="25"/>
+      <c r="D21" s="18"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="28">
         <v>45693</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="28">
         <v>45695</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="19">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="25"/>
+      <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="28">
         <v>45694</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="35">
+      <c r="C26" s="28">
         <v>45699</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="19">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="29">
         <v>45710</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="30">
         <v>45709</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="20">
         <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="31">
         <v>45709</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="31">
         <v>45709</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="38">
+      <c r="C31" s="31">
         <v>45709</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="31">
         <v>45710</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="31">
         <v>45710</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="31">
         <v>45710</v>
       </c>
-      <c r="D34" s="28">
+      <c r="D34" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="31">
         <v>45710</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="31">
         <v>45710</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="31">
         <v>45710</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="31">
         <v>45710</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="39">
+      <c r="C39" s="32">
         <v>45710</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="22">
         <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="39">
+      <c r="C40" s="32">
         <v>45715</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="39">
+      <c r="A41" s="36"/>
+      <c r="B41" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="32">
         <v>45716</v>
       </c>
-      <c r="D41" s="30">
+      <c r="D41" s="23">
         <v>1</v>
       </c>
     </row>
@@ -1311,10 +1316,10 @@
       <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="40">
+      <c r="C42" s="33">
         <v>45715</v>
       </c>
-      <c r="D42" s="31">
+      <c r="D42" s="24">
         <v>3</v>
       </c>
     </row>

</xml_diff>